<commit_message>
Refacoring the CostExporterTest.class - (Task #967)
---
Task #967: Add CostEquipmentWizard
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ImportCostTypeCollectionTest.xlsx
+++ b/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ImportCostTypeCollectionTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\VirtualSatellite4-Core\de.dlr.sc.virsat.model.extension.budget.cost.test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD6FCF2-5079-4C84-998A-76521CE746EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FC654B-D990-4590-9C31-A7EB7E641928}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t xml:space="preserve"> Structural Element UUID</t>
   </si>
@@ -71,24 +71,12 @@
     <t>ea816464-cea3-4db7-ae91-31d37c60a63c</t>
   </si>
   <si>
-    <t>KILL</t>
-  </si>
-  <si>
     <t>1cd42892-eb5f-42ac-881d-e8ef4825254a</t>
   </si>
   <si>
-    <t>FILL</t>
-  </si>
-  <si>
     <t>88544856-794e-49fd-a873-266a4008a3fc</t>
   </si>
   <si>
-    <t>HILL</t>
-  </si>
-  <si>
-    <t>PILL</t>
-  </si>
-  <si>
     <t>505748e0-5d88-47b3-bce8-f53acacb7ccb</t>
   </si>
   <si>
@@ -98,9 +86,6 @@
     <t>13:56 28/7/2016</t>
   </si>
   <si>
-    <t>CostTypeCollection</t>
-  </si>
-  <si>
     <t>VirSat IO Sheet for Cost Types</t>
   </si>
   <si>
@@ -108,6 +93,21 @@
   </si>
   <si>
     <t>CostTypesCollection</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -753,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -772,7 +772,7 @@
     </row>
     <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -802,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" s="9"/>
     </row>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -820,7 +820,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -829,7 +829,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -838,7 +838,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -899,14 +899,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="51.109375" style="2" customWidth="1"/>
     <col min="4" max="256" width="9.109375" customWidth="1"/>
   </cols>
@@ -918,7 +918,7 @@
     </row>
     <row r="2" spans="1:3" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -940,39 +940,39 @@
         <v>13</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="8">
-        <v>1</v>
+      <c r="B5" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed SpotBug in CostExporterTest - (Task #967)
---
Task #967: Add CostEquipmentWizard
</commit_message>
<xml_diff>
--- a/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ImportCostTypeCollectionTest.xlsx
+++ b/de.dlr.sc.virsat.model.extension.budget.cost.test/resources/ImportCostTypeCollectionTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\VirtualSatellite4-Core\de.dlr.sc.virsat.model.extension.budget.cost.test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7D45A0-BC04-46BE-9330-6E481AD6EFBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9CFED1-651E-491C-9796-E012F9FE9A6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="108" windowWidth="20112" windowHeight="9528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,10 +104,10 @@
     <t>X</t>
   </si>
   <si>
-    <t>Entwicklung</t>
-  </si>
-  <si>
     <t>Material</t>
+  </si>
+  <si>
+    <t>Development</t>
   </si>
 </sst>
 </file>
@@ -900,7 +900,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,7 +951,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -972,7 +972,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>